<commit_message>
added data to processed.xlsx
</commit_message>
<xml_diff>
--- a/data/processed_cell_data.xlsx
+++ b/data/processed_cell_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a1800000/Library/CloudStorage/Box-Box/SC2023/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a1800000/Library/CloudStorage/Box-Box/StatCons/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6757A2A1-7BE9-CE40-973B-823422C6B4D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EFDCA6B-1F1F-4A41-89E1-3D36A1937A2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="44800" windowHeight="25200" xr2:uid="{24A8DCC9-A95D-FE48-900E-4FAD50604A0B}"/>
   </bookViews>
@@ -35,12 +35,52 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="8">
+  <si>
+    <t>concentration</t>
+  </si>
+  <si>
+    <t>gene_expression</t>
+  </si>
+  <si>
+    <t>placebo</t>
+  </si>
+  <si>
+    <t>treatment</t>
+  </si>
+  <si>
+    <t>cell lines</t>
+  </si>
+  <si>
+    <t>wild-type</t>
+  </si>
+  <si>
+    <t>cell-type 101</t>
+  </si>
+  <si>
+    <t>activating factor 42</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -66,8 +106,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -382,12 +425,998 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E21FAAEC-E687-494B-A87D-DCCBB16FE57E}">
-  <dimension ref="A1"/>
+  <dimension ref="B4:E92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H81" sqref="H81"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B7" s="1">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B8" s="1">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B9" s="1">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="1">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B11" s="1">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B12" s="1">
+        <v>7</v>
+      </c>
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B13" s="1">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B14" s="1">
+        <v>9</v>
+      </c>
+      <c r="D14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B15" s="1">
+        <v>10</v>
+      </c>
+      <c r="D15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B16" s="1">
+        <v>0</v>
+      </c>
+      <c r="D16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B17" s="1">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B18" s="1">
+        <v>2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B19" s="1">
+        <v>3</v>
+      </c>
+      <c r="D19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B20" s="1">
+        <v>4</v>
+      </c>
+      <c r="D20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B21" s="1">
+        <v>5</v>
+      </c>
+      <c r="D21" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B22" s="1">
+        <v>6</v>
+      </c>
+      <c r="D22" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B23" s="1">
+        <v>7</v>
+      </c>
+      <c r="D23" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B24" s="1">
+        <v>8</v>
+      </c>
+      <c r="D24" t="s">
+        <v>5</v>
+      </c>
+      <c r="E24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B25" s="1">
+        <v>9</v>
+      </c>
+      <c r="D25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B26" s="1">
+        <v>10</v>
+      </c>
+      <c r="D26" t="s">
+        <v>5</v>
+      </c>
+      <c r="E26" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B27" s="1">
+        <v>0</v>
+      </c>
+      <c r="D27" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B28" s="1">
+        <v>1</v>
+      </c>
+      <c r="D28" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B29" s="1">
+        <v>2</v>
+      </c>
+      <c r="D29" t="s">
+        <v>5</v>
+      </c>
+      <c r="E29" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B30" s="1">
+        <v>3</v>
+      </c>
+      <c r="D30" t="s">
+        <v>5</v>
+      </c>
+      <c r="E30" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B31" s="1">
+        <v>4</v>
+      </c>
+      <c r="D31" t="s">
+        <v>5</v>
+      </c>
+      <c r="E31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B32" s="1">
+        <v>5</v>
+      </c>
+      <c r="D32" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B33" s="1">
+        <v>6</v>
+      </c>
+      <c r="D33" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B34" s="1">
+        <v>7</v>
+      </c>
+      <c r="D34" t="s">
+        <v>5</v>
+      </c>
+      <c r="E34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B35" s="1">
+        <v>8</v>
+      </c>
+      <c r="D35" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B36" s="1">
+        <v>9</v>
+      </c>
+      <c r="D36" t="s">
+        <v>5</v>
+      </c>
+      <c r="E36" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B37" s="1">
+        <v>10</v>
+      </c>
+      <c r="D37" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B38" s="1">
+        <v>0</v>
+      </c>
+      <c r="D38" t="s">
+        <v>5</v>
+      </c>
+      <c r="E38" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B39" s="1">
+        <v>1</v>
+      </c>
+      <c r="D39" t="s">
+        <v>5</v>
+      </c>
+      <c r="E39" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B40" s="1">
+        <v>2</v>
+      </c>
+      <c r="D40" t="s">
+        <v>5</v>
+      </c>
+      <c r="E40" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B41" s="1">
+        <v>3</v>
+      </c>
+      <c r="D41" t="s">
+        <v>5</v>
+      </c>
+      <c r="E41" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B42" s="1">
+        <v>4</v>
+      </c>
+      <c r="D42" t="s">
+        <v>5</v>
+      </c>
+      <c r="E42" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B43" s="1">
+        <v>5</v>
+      </c>
+      <c r="D43" t="s">
+        <v>5</v>
+      </c>
+      <c r="E43" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B44" s="1">
+        <v>6</v>
+      </c>
+      <c r="D44" t="s">
+        <v>5</v>
+      </c>
+      <c r="E44" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B45" s="1">
+        <v>7</v>
+      </c>
+      <c r="D45" t="s">
+        <v>5</v>
+      </c>
+      <c r="E45" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B46" s="1">
+        <v>8</v>
+      </c>
+      <c r="D46" t="s">
+        <v>5</v>
+      </c>
+      <c r="E46" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B47" s="1">
+        <v>9</v>
+      </c>
+      <c r="D47" t="s">
+        <v>5</v>
+      </c>
+      <c r="E47" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B48" s="1">
+        <v>10</v>
+      </c>
+      <c r="D48" t="s">
+        <v>5</v>
+      </c>
+      <c r="E48" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B49" s="1">
+        <v>0</v>
+      </c>
+      <c r="D49" t="s">
+        <v>6</v>
+      </c>
+      <c r="E49" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B50" s="1">
+        <v>1</v>
+      </c>
+      <c r="D50" t="s">
+        <v>6</v>
+      </c>
+      <c r="E50" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B51" s="1">
+        <v>2</v>
+      </c>
+      <c r="D51" t="s">
+        <v>6</v>
+      </c>
+      <c r="E51" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B52" s="1">
+        <v>3</v>
+      </c>
+      <c r="D52" t="s">
+        <v>6</v>
+      </c>
+      <c r="E52" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B53" s="1">
+        <v>4</v>
+      </c>
+      <c r="D53" t="s">
+        <v>6</v>
+      </c>
+      <c r="E53" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B54" s="1">
+        <v>5</v>
+      </c>
+      <c r="D54" t="s">
+        <v>6</v>
+      </c>
+      <c r="E54" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B55" s="1">
+        <v>6</v>
+      </c>
+      <c r="D55" t="s">
+        <v>6</v>
+      </c>
+      <c r="E55" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B56" s="1">
+        <v>7</v>
+      </c>
+      <c r="D56" t="s">
+        <v>6</v>
+      </c>
+      <c r="E56" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B57" s="1">
+        <v>8</v>
+      </c>
+      <c r="D57" t="s">
+        <v>6</v>
+      </c>
+      <c r="E57" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B58" s="1">
+        <v>9</v>
+      </c>
+      <c r="D58" t="s">
+        <v>6</v>
+      </c>
+      <c r="E58" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B59" s="1">
+        <v>10</v>
+      </c>
+      <c r="D59" t="s">
+        <v>6</v>
+      </c>
+      <c r="E59" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B60" s="1">
+        <v>0</v>
+      </c>
+      <c r="D60" t="s">
+        <v>6</v>
+      </c>
+      <c r="E60" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B61" s="1">
+        <v>1</v>
+      </c>
+      <c r="D61" t="s">
+        <v>6</v>
+      </c>
+      <c r="E61" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B62" s="1">
+        <v>2</v>
+      </c>
+      <c r="D62" t="s">
+        <v>6</v>
+      </c>
+      <c r="E62" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B63" s="1">
+        <v>3</v>
+      </c>
+      <c r="D63" t="s">
+        <v>6</v>
+      </c>
+      <c r="E63" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B64" s="1">
+        <v>4</v>
+      </c>
+      <c r="D64" t="s">
+        <v>6</v>
+      </c>
+      <c r="E64" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B65" s="1">
+        <v>5</v>
+      </c>
+      <c r="D65" t="s">
+        <v>6</v>
+      </c>
+      <c r="E65" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B66" s="1">
+        <v>6</v>
+      </c>
+      <c r="D66" t="s">
+        <v>6</v>
+      </c>
+      <c r="E66" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B67" s="1">
+        <v>7</v>
+      </c>
+      <c r="D67" t="s">
+        <v>6</v>
+      </c>
+      <c r="E67" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B68" s="1">
+        <v>8</v>
+      </c>
+      <c r="D68" t="s">
+        <v>6</v>
+      </c>
+      <c r="E68" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B69" s="1">
+        <v>9</v>
+      </c>
+      <c r="D69" t="s">
+        <v>6</v>
+      </c>
+      <c r="E69" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B70" s="1">
+        <v>10</v>
+      </c>
+      <c r="D70" t="s">
+        <v>6</v>
+      </c>
+      <c r="E70" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B71" s="1">
+        <v>0</v>
+      </c>
+      <c r="D71" t="s">
+        <v>6</v>
+      </c>
+      <c r="E71" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="72" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B72" s="1">
+        <v>1</v>
+      </c>
+      <c r="D72" t="s">
+        <v>6</v>
+      </c>
+      <c r="E72" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="73" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B73" s="1">
+        <v>2</v>
+      </c>
+      <c r="D73" t="s">
+        <v>6</v>
+      </c>
+      <c r="E73" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="74" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B74" s="1">
+        <v>3</v>
+      </c>
+      <c r="D74" t="s">
+        <v>6</v>
+      </c>
+      <c r="E74" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="75" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B75" s="1">
+        <v>4</v>
+      </c>
+      <c r="D75" t="s">
+        <v>6</v>
+      </c>
+      <c r="E75" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="76" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B76" s="1">
+        <v>5</v>
+      </c>
+      <c r="D76" t="s">
+        <v>6</v>
+      </c>
+      <c r="E76" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="77" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B77" s="1">
+        <v>6</v>
+      </c>
+      <c r="D77" t="s">
+        <v>6</v>
+      </c>
+      <c r="E77" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="78" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B78" s="1">
+        <v>7</v>
+      </c>
+      <c r="D78" t="s">
+        <v>6</v>
+      </c>
+      <c r="E78" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="79" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B79" s="1">
+        <v>8</v>
+      </c>
+      <c r="D79" t="s">
+        <v>6</v>
+      </c>
+      <c r="E79" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="80" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B80" s="1">
+        <v>9</v>
+      </c>
+      <c r="D80" t="s">
+        <v>6</v>
+      </c>
+      <c r="E80" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="81" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B81" s="1">
+        <v>10</v>
+      </c>
+      <c r="D81" t="s">
+        <v>6</v>
+      </c>
+      <c r="E81" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="82" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B82" s="1">
+        <v>0</v>
+      </c>
+      <c r="D82" t="s">
+        <v>6</v>
+      </c>
+      <c r="E82" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="83" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B83" s="1">
+        <v>1</v>
+      </c>
+      <c r="D83" t="s">
+        <v>6</v>
+      </c>
+      <c r="E83" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="84" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B84" s="1">
+        <v>2</v>
+      </c>
+      <c r="D84" t="s">
+        <v>6</v>
+      </c>
+      <c r="E84" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="85" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B85" s="1">
+        <v>3</v>
+      </c>
+      <c r="D85" t="s">
+        <v>6</v>
+      </c>
+      <c r="E85" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="86" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B86" s="1">
+        <v>4</v>
+      </c>
+      <c r="D86" t="s">
+        <v>6</v>
+      </c>
+      <c r="E86" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="87" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B87" s="1">
+        <v>5</v>
+      </c>
+      <c r="D87" t="s">
+        <v>6</v>
+      </c>
+      <c r="E87" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="88" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B88" s="1">
+        <v>6</v>
+      </c>
+      <c r="D88" t="s">
+        <v>6</v>
+      </c>
+      <c r="E88" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="89" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B89" s="1">
+        <v>7</v>
+      </c>
+      <c r="D89" t="s">
+        <v>6</v>
+      </c>
+      <c r="E89" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="90" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B90" s="1">
+        <v>8</v>
+      </c>
+      <c r="D90" t="s">
+        <v>6</v>
+      </c>
+      <c r="E90" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="91" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B91" s="1">
+        <v>9</v>
+      </c>
+      <c r="D91" t="s">
+        <v>6</v>
+      </c>
+      <c r="E91" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="92" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B92" s="1">
+        <v>10</v>
+      </c>
+      <c r="D92" t="s">
+        <v>6</v>
+      </c>
+      <c r="E92" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>